<commit_message>
feat: primeira tela inicial feita com escolha dos jogadores
</commit_message>
<xml_diff>
--- a/documentacao/eap-gantt.xlsx
+++ b/documentacao/eap-gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f958b964552cb1a6/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\tiago\faculdade\gerenciamento-software\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{3187A5D2-2201-4BD4-80BE-FA6C9EEBC8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BE16AFF-9376-4A15-96F4-153D8F005161}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11FB3EB-3100-4D6B-A7F2-8A982AF3FD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{804ACD51-85FD-475A-949B-B4576FE310A5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{804ACD51-85FD-475A-949B-B4576FE310A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planejamento" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="226">
   <si>
     <t>Nível 1</t>
   </si>
@@ -744,6 +744,12 @@
   </si>
   <si>
     <t>Documentação</t>
+  </si>
+  <si>
+    <t>2.2.2.15</t>
+  </si>
+  <si>
+    <t>Criação da Inicialização do Jogo</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1812,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7B9E6FCD-91FA-4847-A1CD-1D89FB9840DD}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="70" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1817,7 +1823,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9633857" cy="5996214"/>
+    <xdr:ext cx="9636824" cy="6006541"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -1844,10 +1850,6 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2149,11 +2151,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC84F76D-DD96-4E1C-B208-4A56AE55DAAE}">
   <dimension ref="A1:AK80"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -11431,6 +11433,24 @@
       </c>
     </row>
     <row r="79" spans="1:37" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="N79" s="1">
         <f>SUM(N2:N78)</f>
         <v>442</v>

</xml_diff>

<commit_message>
Lógica de ataque finalizada
</commit_message>
<xml_diff>
--- a/documentacao/eap-gantt.xlsx
+++ b/documentacao/eap-gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\tiago\faculdade\gerenciamento-software\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11FB3EB-3100-4D6B-A7F2-8A982AF3FD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2B75FE-B28F-4D4D-B77A-52F2CB91668E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{804ACD51-85FD-475A-949B-B4576FE310A5}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="227">
   <si>
     <t>Nível 1</t>
   </si>
@@ -750,6 +750,9 @@
   </si>
   <si>
     <t>Criação da Inicialização do Jogo</t>
+  </si>
+  <si>
+    <t>Criação do WebSocket</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1826,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9636824" cy="6006541"/>
+    <xdr:ext cx="9633857" cy="5996214"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -2152,10 +2155,10 @@
   <dimension ref="A1:AK80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I78" sqref="I78"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4435,7 +4438,7 @@
     </row>
     <row r="20" spans="1:37" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>174</v>
@@ -11537,6 +11540,12 @@
       </c>
     </row>
     <row r="80" spans="1:37" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>19</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="R80" s="8">
         <f>R79/6</f>
         <v>5</v>
@@ -16094,7 +16103,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20">
-        <v>19</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Feat: Calculando a totalidade
</commit_message>
<xml_diff>
--- a/documentacao/eap-gantt.xlsx
+++ b/documentacao/eap-gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\tiago\faculdade\gerenciamento-software\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5658B3-9CDF-40DA-80FA-EFF7301E2FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A861E9A1-E1D4-4AE0-94BA-492C234C82D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{804ACD51-85FD-475A-949B-B4576FE310A5}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="228">
   <si>
     <t>Nível 1</t>
   </si>
@@ -753,6 +753,9 @@
   </si>
   <si>
     <t>Criação do WebSocket</t>
+  </si>
+  <si>
+    <t>Criação da Lógica de Totalidade</t>
   </si>
 </sst>
 </file>
@@ -2152,13 +2155,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC84F76D-DD96-4E1C-B208-4A56AE55DAAE}">
-  <dimension ref="A1:AK80"/>
+  <dimension ref="A1:AK81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -11585,6 +11588,14 @@
       <c r="AA80" s="8">
         <f t="shared" si="24"/>
         <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>